<commit_message>
Update to behavior specification and functional specification to account for latest corrections and resolution of behavioral spec. Basic software architecture defined.
</commit_message>
<xml_diff>
--- a/doc/assurance/ZoneWarningService/5-Issues/issues.xlsx
+++ b/doc/assurance/ZoneWarningService/5-Issues/issues.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dependable/Contracts/ASTRA/Deliverables/OpenUxAS-ZoneAlert/doc/assurance/ZoneWarningService/5-Issues/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9277DC-14E3-5F40-B449-56772AF91356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490F5E86-81D5-BE4C-941C-68958EF8EC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="500" windowWidth="29780" windowHeight="20340" xr2:uid="{C9A58872-7F3C-C947-8C7B-D579EDD417B1}"/>
+    <workbookView xWindow="200" yWindow="500" windowWidth="33760" windowHeight="20740" xr2:uid="{C9A58872-7F3C-C947-8C7B-D579EDD417B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>Status</t>
   </si>
@@ -110,6 +110,99 @@
   </si>
   <si>
     <t>Documented in specification</t>
+  </si>
+  <si>
+    <t>There is a fixed constant buffering size in the vehicle path planning. Should we apply this same constant buffer, or make it a parameter of the service? Ask Sean if he has an opinion.</t>
+  </si>
+  <si>
+    <t>CMASI:AbstractZone has a padding attribute that defaults to zero. This padding vavlue is a standin for a vehicle radius + any additional semantics to buffer extra padding around zone boundaries</t>
+  </si>
+  <si>
+    <t>Need to write a design constraint requirement of the system that it re-use the polygon structure already present in OpenUxAS</t>
+  </si>
+  <si>
+    <t>OK. Use zone padding. Make a requirement that the ZoneAlertService re-use polygon models from route service. This is now sub-issue 1.20. This will maintain common semantics as well as allow both to use a hardened code base. Consider as opposed to re-doing geometry which might provide error detection in diversity between the two polygon solutions but might also contain common errors (see Knight and Levison result).</t>
+  </si>
+  <si>
+    <t>Question: Modify behavior and functional spec to use zone padding rather than vehicle radius? Force our service to use the same data structures as the existing service, so that padding is always semantically equivalent? Ultimately, what does the visbility graph use? Also, When is it applied. In polygons or in some lower-level data structure? Determining this is sub-issue 1.10.</t>
+  </si>
+  <si>
+    <t>Asking Sean</t>
+  </si>
+  <si>
+    <t>AbstractZone data has minimum and maximum altitudes for zones. Are those in use and are they in scope for our work? What about temporal data in AbstractZones as well?</t>
+  </si>
+  <si>
+    <t>Need to determine if padding from zones as declared is actually used by route planning service. What paadding is used? Where is it used? In polygon model or in some lower-level data structure?</t>
+  </si>
+  <si>
+    <t>Investigating the source code. We can see the padding data is being passed to CPolygon class constructor where it goes into the AbstractZone constructor. I need to get a hold of AbstractZone.h. Found it on virtual machine where LMCP message classes were built. There is a getter getPadding() that I can search for. The visibiliry graph setup algorithms do pass this data, now I remember. THey get the padding, but I'm still following to see if it is used. The non-visibility graph version of the algorith does  store padding as well, checking that it grows reagions for keep-outs and shrinks for keep in. So some semantic checking there. But looking further in the code for the Visilibility Version of the system, Keep In Zones have their padding overridden with zero in a work queue and a comment says "no expansion or shrinking"! In contrast keep out boundaries are allowed to have &gt; 0 padding pass through, but shrinking is disallowed in the code. The actual expansion code for keep out zones is somewhat complex and uses bevelling edges depending on the angle of interactin of two consecutive edges. But basically for each polygon, it puts a rectangle around each edge and then merges those polygons together. The resulting polygon, with some additional bevelling polygons in there, is the puffed up keep-out zone. Oh boy. That semantics is a bit tricky!</t>
+  </si>
+  <si>
+    <t>Sean says this is not used by services that he knows of. It is not used by route planning, and we will follow that semantics. I will make a note that nothing but 2d is used for zones in behavior and specification documents, and also make clear that we follow the semantics used in the route planner service interpretation of zones. no temporal aspects, no lists of vehicle IDs that it applies to.</t>
+  </si>
+  <si>
+    <t>In summary: both versions of route planning service use padding, but differ in the resulting usage. Both will ingore padding that defines a shrink of a keep-out zone or growth of a keep in-zone. Such padding is ignored and the zone polygon set up instead with zero padding. One system enforces growth on keep-out zones and enforces no shrink padding on keep-in zones. The other enforces growth on keep-out zones and shrink on keep-in zones.</t>
+  </si>
+  <si>
+    <t>Documents are updated to reflect the resulting  design change, the issue is now closed.</t>
+  </si>
+  <si>
+    <t>Behavior document states that violation notifications for a vehicle will not be sent if a vehicle is within distance Ed of its planned route at last position report. This is erroneous, it would be better behavior to base this on projected current position relative to the path. Thus, if the state report is very stale, and projected time on linear trajectory would assume the vehicle has drifted from the route, it should report the potential violation. This way, path sensativity is sensative to the staleness of state reports relative to the route curvature.</t>
+  </si>
+  <si>
+    <t>Resolved, behavior document and functional specification altered accordingly.</t>
+  </si>
+  <si>
+    <t>Behavior document erroneously states messages will and will not be resent for the same zone violation by the same aircraft as predicted or occcuring presently for the given aircraft.</t>
+  </si>
+  <si>
+    <t>Fixed to be consistent with the desired behavior of always resending messages based on current data and computation of the service</t>
+  </si>
+  <si>
+    <t>Decide if we want a strongly-coupled re-use of code or a weakly-coupled re-use of a refactored sub-service to compute actual zone polygons from reported zones</t>
+  </si>
+  <si>
+    <t>What is the interaction of projected future violation notifications and current notifications? In the  0.3 behavior document, it is now clear that different semantics for projection of future and current violations might require order of precedence for reporting or not reporting one or both types. Define in the document.</t>
+  </si>
+  <si>
+    <t>Defined a clear definition of how the services might interact in version 0.5 of the document</t>
+  </si>
+  <si>
+    <t>The intiital definition did not pass review, as a case of interest was raised where there is a future time violation of the current path after a part of the path would not be in violation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The chosen rules are maintained and the case that may be of concern is presented to the reader. </t>
+  </si>
+  <si>
+    <t>Review case with stakeholders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on the results of issues  1.10 and 1.20, we need to update the behavior document (Issue 1.3) and and functional specification (Issue 1.4) to apply zone buffering and not vehicle radius.  </t>
+  </si>
+  <si>
+    <t>Behavior document must be updated to reflect use of the zone buffer concept rather than vehicle radius.</t>
+  </si>
+  <si>
+    <t>Functional specificaiton document must be updated to reflext use of the zone buffer concept rather than vehicle radius.</t>
+  </si>
+  <si>
+    <t>Behavior document was updated to reflect use of zone buffer size rather than vehicle collsion radius.</t>
+  </si>
+  <si>
+    <t>Staekholders accept a threshold function that determines earliest possible violation only</t>
+  </si>
+  <si>
+    <t>Put all the documentation in a subservice directory in an isolated place not pollute the main do directoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move docs under a C++ service directory to not pollute </t>
+  </si>
+  <si>
+    <t>Updated and completed</t>
+  </si>
+  <si>
+    <t>1.3 and 1.4 are resolved, therefore this issue is resolved.</t>
   </si>
 </sst>
 </file>
@@ -117,7 +210,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -196,23 +289,10 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -222,18 +302,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,252 +643,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50891FDD-30FA-7E4F-8B50-3438F693C3DF}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="10" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="4" width="47.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="27.83203125" style="11" customWidth="1"/>
+    <col min="3" max="4" width="47.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="76" style="6" customWidth="1"/>
     <col min="9" max="9" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="6" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="3">
         <v>45311</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="8">
+      <c r="F3" s="8">
+        <v>45322</v>
+      </c>
+      <c r="G3" s="4">
         <v>45315</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="13"/>
-      <c r="G4" s="8">
+    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="G4" s="4">
         <v>45315</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="G5" s="4">
+        <v>45316</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="G6" s="4">
+        <v>45317</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="G7" s="4">
+        <v>45317</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="G8" s="4">
+        <v>45320</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="G9" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10" s="4">
+        <v>45322</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G11" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E12" s="4">
         <v>45311</v>
       </c>
-      <c r="G6" s="8">
+      <c r="F12" s="9">
         <v>45316</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="G12" s="4">
+        <v>4</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="D7" s="15"/>
-      <c r="E7" s="13"/>
-      <c r="G7" s="8">
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="G13" s="4">
         <v>45316</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="D8" s="15"/>
-      <c r="E8" s="13"/>
-      <c r="H8" s="11" t="s">
+      <c r="I13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="H14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E15" s="4">
         <v>45311</v>
       </c>
-      <c r="G9" s="8">
+      <c r="F15" s="9">
         <v>45316</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="G15" s="4">
+        <v>45316</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="D10" s="15"/>
-      <c r="E10" s="13"/>
-      <c r="H10" s="11" t="s">
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G16" s="4">
+        <v>45316</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="119" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
         <v>4</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E17" s="4">
         <v>45311</v>
       </c>
-      <c r="G11" s="8">
+      <c r="F17" s="9">
         <v>45316</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="G17" s="4">
+        <v>45316</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="8">
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G18" s="4">
         <v>45316</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="13"/>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="4">
+        <v>45320</v>
+      </c>
+      <c r="F19" s="9">
+        <v>45321</v>
+      </c>
+      <c r="G19" s="4">
+        <v>45320</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="G20" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="4">
+        <v>45320</v>
+      </c>
+      <c r="G21" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="4">
+        <v>45320</v>
+      </c>
+      <c r="F22" s="9">
+        <v>45320</v>
+      </c>
+      <c r="G22" s="4">
+        <v>45320</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="G23" s="4">
+        <v>45320</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45321</v>
+      </c>
+      <c r="F24" s="9">
+        <v>45321</v>
+      </c>
+      <c r="G24" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="4">
+        <v>45321</v>
+      </c>
+      <c r="G25" s="4">
+        <v>45322</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="4">
+        <v>45321</v>
+      </c>
+      <c r="F26" s="9">
+        <v>45321</v>
+      </c>
+      <c r="G26" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="4">
+        <v>45321</v>
+      </c>
+      <c r="F27" s="9">
+        <v>45321</v>
+      </c>
+      <c r="G27" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+      <c r="A28" s="10">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="4">
+        <v>45321</v>
+      </c>
+      <c r="F28" s="9">
+        <v>45321</v>
+      </c>
+      <c r="G28" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="G29" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="G30" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G31" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G32" s="4">
+        <v>45321</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="10">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -805,6 +1237,15 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D1:D2"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="formula" val="&quot;OPEN&quot;" gte="0"/>
+        <cfvo type="formula" val="&quot;RESOLVED&quot;"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>